<commit_message>
Allow for Sector when allocating budget.
</commit_message>
<xml_diff>
--- a/Uganda/Architecture.xlsx
+++ b/Uganda/Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\Q\Uganda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E38B160-2422-4F4F-8E83-0E42A30838C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72558E03-EE95-41B8-8A64-963C7C5012F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{19EBA273-2EE5-46C3-BADC-40EAD78B72AB}"/>
+    <workbookView xWindow="-165" yWindow="150" windowWidth="12405" windowHeight="13050" xr2:uid="{19EBA273-2EE5-46C3-BADC-40EAD78B72AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -358,10 +358,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -690,7 +690,7 @@
   <dimension ref="B2:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +777,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>3</v>
@@ -813,7 +813,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="9">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>3</v>
@@ -849,7 +849,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="9">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>3</v>
@@ -885,7 +885,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="9">
-        <v>4</v>
+        <v>10000</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>3</v>
@@ -921,7 +921,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="9">
-        <v>5</v>
+        <v>100000</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>3</v>
@@ -957,7 +957,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="9">
-        <v>6</v>
+        <v>1000000</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>3</v>
@@ -993,7 +993,7 @@
         <v>14</v>
       </c>
       <c r="F10" s="9">
-        <v>7</v>
+        <v>10000000</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>3</v>
@@ -1029,7 +1029,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="10">
-        <v>8</v>
+        <v>100000000</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>3</v>
@@ -1060,7 +1060,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="11">
         <f>SUM(F4:F11)</f>
-        <v>36</v>
+        <v>111111110</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>9</v>

</xml_diff>